<commit_message>
every basic part has been built,then need to build the top and the testbench
</commit_message>
<xml_diff>
--- a/document/31条指令操作时间表.xlsx
+++ b/document/31条指令操作时间表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\cpu31\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9549762F-AFA9-4B03-8D96-680139AC8BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07A1178-57BE-4047-8E44-FDF06B86B0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{7CAB809C-24DC-4464-89F1-2B336DD29E79}"/>
   </bookViews>
@@ -514,7 +514,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -531,9 +531,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -856,7 +853,7 @@
       <pane xSplit="11" ySplit="16" topLeftCell="L17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1055,7 +1052,7 @@
       <c r="S20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="T20" s="6" t="s">
+      <c r="T20" s="3" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1587,7 +1584,7 @@
         <v>60</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>62</v>
@@ -1649,7 +1646,7 @@
         <v>60</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>62</v>
@@ -1897,7 +1894,7 @@
         <v>60</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>62</v>
@@ -1959,7 +1956,7 @@
         <v>60</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>62</v>
@@ -2021,7 +2018,7 @@
         <v>60</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>62</v>
@@ -2703,7 +2700,7 @@
         <v>60</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>62</v>
@@ -2765,7 +2762,7 @@
         <v>60</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>62</v>

</xml_diff>